<commit_message>
modificando ejemplos TEI 0.2.1
</commit_message>
<xml_diff>
--- a/fhir/ig/tei/0.2.1/CodeSystem-CSConsecuenciaAtencionCodigo.xlsx
+++ b/fhir/ig/tei/0.2.1/CodeSystem-CSConsecuenciaAtencionCodigo.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>Property</t>
   </si>
@@ -490,7 +490,9 @@
       <c r="C2" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" t="s" s="2">
+        <v>41</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
@@ -502,7 +504,9 @@
       <c r="C3" t="s" s="2">
         <v>43</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" t="s" s="2">
+        <v>43</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
@@ -514,7 +518,9 @@
       <c r="C4" t="s" s="2">
         <v>44</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" t="s" s="2">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>